<commit_message>
settelment as comment of amr 15/8/2018
modification in a source code in this point: in text attached

I have some question to bank
1- Reconciliation amount mean sum of sale or what ??
2- Fields 75, 76,77,83,84,86,87,88,89, 97  (Sum of all the financial transactions in which the positions 1-2 of processing code inside the financial transaction indicated debit.)
I have the total for
a- sale
b- refund
c- void sale
d- void refund
please map fields with total or describe the calculation of every field
3- please describe statement ( processing code inside the financial transaction indicated debit or credit in another field)
4- in field 55 will send data for ICC only

I have some question for John
1- how to get EMV data and put in s_icc_data.w_misc_len and format tags as a specification in field 55 (HPS Document)
</commit_message>
<xml_diff>
--- a/File/fields_number_byte.xlsx
+++ b/File/fields_number_byte.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmedhamed\Documents\GitHub\S_MISR\File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bank Miser\Core\S_MISR\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>